<commit_message>
Mise à Jour des Excels
Ajout des graphiques des excels de nouvelle ligne de notation et et remise en page
</commit_message>
<xml_diff>
--- a/Grille_d_evaluation_Ma_Cyber_Auto_Entreprise.xlsx
+++ b/Grille_d_evaluation_Ma_Cyber_Auto_Entreprise.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EBAAA8-6550-4A40-861C-A1998E461AE2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB92978-DC6E-4A77-BEAF-0F1E478A5DC6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,15 +14,49 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">[1]Feuil1!$B$5</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">[1]Feuil1!$C$4:$G$4</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">[1]Feuil1!$C$5:$G$5</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">[1]Feuil1!$B$7</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">[1]Feuil1!$C$4:$G$4</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">[1]Feuil1!$C$7:$G$7</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Feuil1!$B$7</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Feuil1!$C$4:$G$4</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">[1]Feuil1!$C$4:$G$4</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">[1]Feuil1!$C$7:$G$7</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">[1]Feuil1!$B$5</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">[1]Feuil1!$C$4:$G$4</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">[1]Feuil1!$C$5:$G$5</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">[1]Feuil1!$B$11</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">[1]Feuil1!$C$11:$G$11</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">[1]Feuil1!$C$4:$G$4</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">[1]Feuil1!$B$8</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">[1]Feuil1!$C$4:$G$4</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Feuil1!$C$7:$G$7</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">[1]Feuil1!$C$8:$G$8</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">[1]Feuil1!$B$9</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">[1]Feuil1!$C$4:$G$4</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">[1]Feuil1!$C$9:$G$9</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Feuil1!$V$20</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">[1]Feuil1!$B$10</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">[1]Feuil1!$C$10:$G$10</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">[1]Feuil1!$C$4:$G$4</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">[1]Feuil1!$B$7</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">[1]Feuil1!$C$4:$G$4</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Feuil1!$B$10</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">[1]Feuil1!$C$7:$G$7</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">Feuil1!$B$8</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">Feuil1!$C$4:$G$4</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">Feuil1!$C$8:$G$8</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">Feuil1!$B$9</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">Feuil1!$C$4:$G$4</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">Feuil1!$C$9:$G$9</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">Feuil1!$B$11</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">Feuil1!$C$11:$G$11</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">Feuil1!$C$4:$G$4</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Feuil1!$C$10:$G$10</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">Feuil1!$B$11</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">Feuil1!$C$11:$G$11</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">Feuil1!$C$4:$G$4</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Feuil1!$C$4:$G$4</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">[1]Feuil1!$B$6</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">[1]Feuil1!$C$4:$G$4</definedName>
     <definedName name="_xlchart.v1.8" hidden="1">[1]Feuil1!$C$6:$G$6</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">[1]Feuil1!$B$7</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Note (5 plus positif, 1 plus négatif 
 exmple : 5=intention parfaitement comprise, 1 intention non comprise)</t>
@@ -73,15 +107,8 @@
     <t>Age :</t>
   </si>
   <si>
-    <t>Métier/étude:</t>
-  </si>
-  <si>
     <t>Fréquence
  de jeu :</t>
-  </si>
-  <si>
-    <t>Fréquence d'utilisation
-d'internet :</t>
   </si>
   <si>
     <t>//Souhaite 
@@ -94,14 +121,7 @@
     <t>Femme</t>
   </si>
   <si>
-    <t>vendeuse en
- boulangerie</t>
-  </si>
-  <si>
     <t>très rarement</t>
-  </si>
-  <si>
-    <t>tout les jours</t>
   </si>
   <si>
     <t>Laura</t>
@@ -120,12 +140,34 @@
     <t>Homme</t>
   </si>
   <si>
-    <t>2ème année en fac 
-de math</t>
+    <t>Plusieurs heurs 
+par semaines</t>
   </si>
   <si>
-    <t>Plusieurs heurs 
-par semaines</t>
+    <t>Les commandes du jeu ont été comprise</t>
+  </si>
+  <si>
+    <t>Les joueurs on atteints les objectifs du jeu</t>
+  </si>
+  <si>
+    <t>Les joueurs ont lu tout le texte</t>
+  </si>
+  <si>
+    <t>commentaire</t>
+  </si>
+  <si>
+    <t>Métier/Etudes</t>
+  </si>
+  <si>
+    <t>vendeuse en 
+boulangerie</t>
+  </si>
+  <si>
+    <t>2ième année 
+fac de math</t>
+  </si>
+  <si>
+    <t>Les joueurs en ont appris plus sur l'auto entrepreunariat</t>
   </si>
 </sst>
 </file>
@@ -148,18 +190,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -210,7 +246,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -225,7 +261,244 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -237,11 +510,50 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -259,11 +571,13 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -272,12 +586,21 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -291,19 +614,17 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -312,25 +633,32 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -340,274 +668,199 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -616,6 +869,15 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9933"/>
+      <color rgb="FFFFFF00"/>
+      <color rgb="FF99FF33"/>
+      <color rgb="FF66FF33"/>
+      <color rgb="FFFF6600"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -632,10 +894,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f dir="row">_xlchart.v1.1</cx:f>
+        <cx:f dir="row">_xlchart.v1.13</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f dir="row">_xlchart.v1.2</cx:f>
+        <cx:f dir="row">_xlchart.v1.14</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -673,7 +935,7 @@
         <cx:series layoutId="sunburst" uniqueId="{D8D479D4-D5E3-4AB5-8424-DDD270067037}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:f>_xlchart.v1.12</cx:f>
               <cx:v>Intention comprise 
 par les joueurs</cx:v>
             </cx:txData>
@@ -855,10 +1117,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f dir="row">_xlchart.v1.4</cx:f>
+        <cx:f dir="row">_xlchart.v1.1</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f dir="row">_xlchart.v1.5</cx:f>
+        <cx:f dir="row">_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -866,7 +1128,7 @@
     <cx:title pos="t" align="ctr" overlay="0">
       <cx:tx>
         <cx:txData>
-          <cx:v>Mécaniques comprise</cx:v>
+          <cx:v>Mécaniques comprises</cx:v>
         </cx:txData>
       </cx:tx>
       <cx:txPr>
@@ -877,26 +1139,26 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="fr-FR" sz="1800" b="1" i="0" u="none" strike="noStrike" cap="all" spc="150" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:sysClr>
               </a:solidFill>
               <a:latin typeface="Calibri" panose="020F0502020204030204"/>
             </a:rPr>
-            <a:t>Mécaniques comprise</a:t>
+            <a:t>Mécaniques comprises</a:t>
           </a:r>
         </a:p>
       </cx:txPr>
     </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="sunburst" uniqueId="{D13C0031-F218-4A63-AC20-099A35C99884}">
+        <cx:series layoutId="sunburst" uniqueId="{B3490342-7905-439C-9D79-5EB61B95A11E}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.3</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>Les mécaniques ont été comprises</cx:v>
             </cx:txData>
           </cx:tx>
@@ -910,7 +1172,7 @@
           <cx:dataPt idx="1">
             <cx:spPr>
               <a:solidFill>
-                <a:srgbClr val="CCFF33"/>
+                <a:srgbClr val="99FF33"/>
               </a:solidFill>
             </cx:spPr>
           </cx:dataPt>
@@ -931,7 +1193,395 @@
           <cx:dataPt idx="4">
             <cx:spPr>
               <a:solidFill>
-                <a:srgbClr val="FF3300"/>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataLabels pos="ctr">
+            <cx:visibility seriesName="0" categoryName="1" value="0"/>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx4.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f dir="row">_xlchart.v1.32</cx:f>
+      </cx:strDim>
+      <cx:numDim type="size">
+        <cx:f dir="row">_xlchart.v1.33</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Commandes comprises</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1800" b="1" i="0" u="none" strike="noStrike" cap="all" spc="150" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Commandes comprises</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="sunburst" uniqueId="{2A62DF3B-3F14-4BCC-A8FC-D1AD57351E82}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.31</cx:f>
+              <cx:v>Les commandes du jeu ont été comprise</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataPt idx="0">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="66FF33"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataPt idx="1">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="99FF33"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataPt idx="2">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataPt idx="3">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF9933"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataPt idx="4">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataLabels pos="ctr">
+            <cx:visibility seriesName="0" categoryName="1" value="0"/>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx5.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f dir="row">_xlchart.v1.35</cx:f>
+      </cx:strDim>
+      <cx:numDim type="size">
+        <cx:f dir="row">_xlchart.v1.36</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Les joueurs ont appris sur l'auto entrepreunariat</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1800" b="1" i="0" u="none" strike="noStrike" cap="all" spc="150" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Les joueurs ont appris sur l'auto entrepreunariat</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="sunburst" uniqueId="{943DF8EE-CD8C-42AF-BE52-C38226F0E488}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.34</cx:f>
+              <cx:v>Les joueurs en ont appris plus sur l'auto entrepreunariat</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataPt idx="0">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="66FF33"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataPt idx="1">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="99FF33"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataPt idx="2">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataPt idx="3">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF9933"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataPt idx="4">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataLabels pos="ctr">
+            <cx:visibility seriesName="0" categoryName="1" value="0"/>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx6.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f dir="row">_xlchart.v1.5</cx:f>
+      </cx:strDim>
+      <cx:numDim type="size">
+        <cx:f dir="row">_xlchart.v1.4</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Objectifs du jeu atteints</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1800" b="1" i="0" u="none" strike="noStrike" cap="all" spc="150" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Objectifs du jeu atteints</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="sunburst" uniqueId="{79916366-4609-4AE5-8653-538F9E51AAF7}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.3</cx:f>
+              <cx:v>Les joueurs on atteints les objectifs du jeu</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataPt idx="0">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="66FF33"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataPt idx="1">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="99FF33"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataPt idx="2">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataPt idx="3">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF9933"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataPt idx="4">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataLabels pos="ctr">
+            <cx:visibility seriesName="0" categoryName="1" value="0"/>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx7.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f dir="row">_xlchart.v1.39</cx:f>
+      </cx:strDim>
+      <cx:numDim type="size">
+        <cx:f dir="row">_xlchart.v1.38</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>on lu tout le texte</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1800" b="1" i="0" u="none" strike="noStrike" cap="all" spc="150" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>on lu tout le texte</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="sunburst" uniqueId="{9914D138-9446-4419-AC22-5A7A737F9146}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.37</cx:f>
+              <cx:v>Les joueurs ont lu tout le texte</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataPt idx="0">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="66FF33"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataPt idx="1">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="99FF33"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataPt idx="2">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataPt idx="3">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF9933"/>
+              </a:solidFill>
+            </cx:spPr>
+          </cx:dataPt>
+          <cx:dataPt idx="4">
+            <cx:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </cx:spPr>
           </cx:dataPt>
@@ -1067,6 +1717,166 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="382">
   <cs:axisTitle>
@@ -2148,6 +2958,2166 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="382">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr lIns="38100" tIns="19050" rIns="38100" bIns="19050">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" cap="all" spc="150"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="382">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr lIns="38100" tIns="19050" rIns="38100" bIns="19050">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" cap="all" spc="150"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="382">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr lIns="38100" tIns="19050" rIns="38100" bIns="19050">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" cap="all" spc="150"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="382">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr lIns="38100" tIns="19050" rIns="38100" bIns="19050">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" cap="all" spc="150"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="382">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2694,13 +5664,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:rowOff>4763</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -2736,8 +5706,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5476875" y="395287"/>
-              <a:ext cx="4572000" cy="3676650"/>
+              <a:off x="7867650" y="1157288"/>
+              <a:ext cx="3057525" cy="4776788"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2769,16 +5739,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -2814,8 +5784,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5467350" y="4233862"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="11496675" y="1138237"/>
+              <a:ext cx="3076575" cy="4795838"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2849,23 +5819,23 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>933449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>695324</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="4" name="Graphique 3">
+            <xdr:cNvPr id="11" name="Graphique 10">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B76BB66-29AF-45DC-8FC2-47C0848E37BB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5D48C92-047C-4EAF-A2CD-5119B222F2D6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2892,8 +5862,320 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5476875" y="7110412"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="7867650" y="6848474"/>
+              <a:ext cx="3067050" cy="4752975"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="fr-FR" sz="1100"/>
+                <a:t>Ce graphique n’est pas disponible dans votre version d’Excel.
+La modification de cette forme ou l’enregistrement de ce classeur dans un autre format de fichier endommagera le graphique de façon irréparable.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>704850</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="12" name="Graphique 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F611DEF4-ABC2-4E54-BE96-DFBB9B27E725}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11534774" y="6867525"/>
+              <a:ext cx="3048001" cy="4743450"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="fr-FR" sz="1100"/>
+                <a:t>Ce graphique n’est pas disponible dans votre version d’Excel.
+La modification de cette forme ou l’enregistrement de ce classeur dans un autre format de fichier endommagera le graphique de façon irréparable.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="13" name="Graphique 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A6F9EA3-F01D-4D9E-93F6-2EBADAAFC5B2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7872412" y="12582525"/>
+              <a:ext cx="3043238" cy="4743450"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="fr-FR" sz="1100"/>
+                <a:t>Ce graphique n’est pas disponible dans votre version d’Excel.
+La modification de cette forme ou l’enregistrement de ce classeur dans un autre format de fichier endommagera le graphique de façon irréparable.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>942974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>942974</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="14" name="Graphique 13">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CFDC8A0-A202-46D2-9CDB-8508224220EC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11525250" y="12563474"/>
+              <a:ext cx="3057525" cy="4752975"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="fr-FR" sz="1100"/>
+                <a:t>Ce graphique n’est pas disponible dans votre version d’Excel.
+La modification de cette forme ou l’enregistrement de ce classeur dans un autre format de fichier endommagera le graphique de façon irréparable.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>576262</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="16" name="Graphique 15">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFAB18B4-4B17-4F81-9A1D-B2E93D3F804F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7843837" y="18307049"/>
+              <a:ext cx="3062288" cy="4219575"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3010,6 +6292,86 @@
             <v>1</v>
           </cell>
           <cell r="G7">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8" t="str">
+            <v>Les commandes du jeu ont été comprise</v>
+          </cell>
+          <cell r="C8">
+            <v>1</v>
+          </cell>
+          <cell r="D8">
+            <v>1</v>
+          </cell>
+          <cell r="E8">
+            <v>1</v>
+          </cell>
+          <cell r="F8">
+            <v>1</v>
+          </cell>
+          <cell r="G8">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9" t="str">
+            <v>Les joueurs en ont appris plus sur la manipulation d'informations</v>
+          </cell>
+          <cell r="C9">
+            <v>1</v>
+          </cell>
+          <cell r="D9">
+            <v>1</v>
+          </cell>
+          <cell r="E9">
+            <v>1</v>
+          </cell>
+          <cell r="F9">
+            <v>1</v>
+          </cell>
+          <cell r="G9">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10" t="str">
+            <v>Les joueurs on atteints les objectifs du jeu</v>
+          </cell>
+          <cell r="C10">
+            <v>1</v>
+          </cell>
+          <cell r="D10">
+            <v>1</v>
+          </cell>
+          <cell r="E10">
+            <v>1</v>
+          </cell>
+          <cell r="F10">
+            <v>1</v>
+          </cell>
+          <cell r="G10">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11" t="str">
+            <v>Les joueurs ont lu tout le texte</v>
+          </cell>
+          <cell r="C11">
+            <v>1</v>
+          </cell>
+          <cell r="D11">
+            <v>1</v>
+          </cell>
+          <cell r="E11">
+            <v>1</v>
+          </cell>
+          <cell r="F11">
+            <v>1</v>
+          </cell>
+          <cell r="G11">
             <v>1</v>
           </cell>
         </row>
@@ -3282,309 +6644,396 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q18"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q34" sqref="Q34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="8" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="8" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:17" s="25" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="22"/>
-      <c r="C3" s="24" t="s">
+    <row r="3" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="55"/>
+      <c r="C3" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="26" t="s">
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="41" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="23"/>
-      <c r="C4" s="3">
+    <row r="4" spans="1:17" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="56"/>
+      <c r="C4" s="52">
         <v>5</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="5">
         <v>4</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="6">
         <v>3</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="7">
         <v>2</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="49">
         <v>1</v>
       </c>
-      <c r="H4" s="27"/>
+      <c r="H4" s="50"/>
     </row>
-    <row r="5" spans="1:17" ht="75" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+    <row r="5" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="53">
         <v>1</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="44">
         <v>1</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="45">
         <v>1</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="46">
         <v>1</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="47">
         <v>1</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="48">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="60" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+    <row r="6" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="29">
         <v>1</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="2">
         <v>1</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="3">
         <v>1</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="4">
         <v>1</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="27">
         <v>1</v>
       </c>
-      <c r="H6" s="29"/>
+      <c r="H6" s="42"/>
     </row>
-    <row r="7" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="14" t="s">
+    <row r="7" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="29">
         <v>1</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="2">
         <v>1</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="3">
         <v>1</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="4">
         <v>1</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="27">
         <v>1</v>
       </c>
-      <c r="H7" s="30"/>
-      <c r="K7" s="20"/>
+      <c r="H7" s="42"/>
+      <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="31" t="s">
+    <row r="8" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="29">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="27">
+        <v>1</v>
+      </c>
+      <c r="H8" s="42"/>
+    </row>
+    <row r="9" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="29">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="27">
+        <v>1</v>
+      </c>
+      <c r="H9" s="42"/>
+    </row>
+    <row r="10" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="29">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1</v>
+      </c>
+      <c r="G10" s="27">
+        <v>1</v>
+      </c>
+      <c r="H10" s="42"/>
+    </row>
+    <row r="11" spans="1:17" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="54">
+        <v>1</v>
+      </c>
+      <c r="D11" s="34">
+        <v>1</v>
+      </c>
+      <c r="E11" s="35">
+        <v>1</v>
+      </c>
+      <c r="F11" s="36">
+        <v>1</v>
+      </c>
+      <c r="G11" s="40">
+        <v>1</v>
+      </c>
+      <c r="H11" s="43"/>
+    </row>
+    <row r="12" spans="1:17" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="38"/>
+    </row>
+    <row r="13" spans="1:17" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H13" s="23"/>
+    </row>
+    <row r="14" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="26"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="23"/>
     </row>
-    <row r="10" spans="1:17" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="33" t="s">
+    <row r="15" spans="1:17" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C15" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D15" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E15" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="34" t="s">
+      <c r="F15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="35" t="s">
+      <c r="G15" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="23"/>
+    </row>
+    <row r="16" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="36" t="s">
+      <c r="C16" s="14" t="s">
         <v>13</v>
       </c>
+      <c r="D16" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="23"/>
     </row>
-    <row r="11" spans="1:17" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="37" t="s">
+    <row r="17" spans="2:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="15"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="23"/>
+    </row>
+    <row r="18" spans="2:8" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="15"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="23"/>
+    </row>
+    <row r="19" spans="2:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
+    </row>
+    <row r="20" spans="2:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="38" t="s">
+      <c r="E20" s="16">
         <v>16</v>
       </c>
-      <c r="E11" s="38"/>
-      <c r="F11" s="39" t="s">
+      <c r="F20" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="40" t="s">
+    </row>
+    <row r="21" spans="2:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="17"/>
+    </row>
+    <row r="22" spans="2:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="15"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="17"/>
+    </row>
+    <row r="23" spans="2:8" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="41"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="43"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="41"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="43"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="41"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="43"/>
-    </row>
-    <row r="15" spans="1:17" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="42" t="s">
+      <c r="D23" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="42">
-        <v>16</v>
-      </c>
-      <c r="F15" s="42" t="s">
+      <c r="E23" s="21">
+        <v>19</v>
+      </c>
+      <c r="F23" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="45" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="40" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="41"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="43"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="41"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="43"/>
-    </row>
-    <row r="18" spans="2:8" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="47" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="47">
-        <v>19</v>
-      </c>
-      <c r="F18" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="H18" s="21" t="s">
-        <v>19</v>
+      <c r="G23" s="61" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="H5:H11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="B14:G14"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="H3:H4"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B9:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>